<commit_message>
Hoy si commit final de las graficas
</commit_message>
<xml_diff>
--- a/src/Graficas Profiler.xlsx
+++ b/src/Graficas Profiler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. UVG Tercer semestre\Algoritmos y estructura de datos\HT3\HojaDeTrabajo3\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CD9A54-012C-46A6-8E9E-07267D7F6121}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDDCCFC4-590E-4DAB-924C-B2EE4FFDAEE2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6FAA0B11-C541-4B78-A08C-0A0B67013B6B}"/>
   </bookViews>
@@ -72,7 +72,7 @@
     <t>Profiler utilizado</t>
   </si>
   <si>
-    <t>mediante Triggers</t>
+    <t>Integracion de intellij y jprofiler, tiempos mediante triggers</t>
   </si>
 </sst>
 </file>
@@ -157,7 +157,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -168,6 +168,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -6102,10 +6105,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{211EB932-C3FD-4F1E-9249-C9A647314BEC}">
-  <dimension ref="B1:O45"/>
+  <dimension ref="B1:O46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T45" sqref="T45"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45:O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6732,17 +6735,27 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="45" spans="10:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="10:15" x14ac:dyDescent="0.3">
       <c r="J45" t="s">
         <v>12</v>
       </c>
-      <c r="L45" t="s">
+      <c r="L45" s="10" t="s">
         <v>13</v>
       </c>
+      <c r="M45" s="10"/>
+      <c r="N45" s="10"/>
+      <c r="O45" s="10"/>
+    </row>
+    <row r="46" spans="10:15" x14ac:dyDescent="0.3">
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C1:O2"/>
+    <mergeCell ref="L45:O46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>